<commit_message>
Uploading Changes in Project: Pass Impressions Jasper Service Impression Service
</commit_message>
<xml_diff>
--- a/src/informesGenerados/HechosParaUnidadOrganizativa.xlsx
+++ b/src/informesGenerados/HechosParaUnidadOrganizativa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>UOrg</t>
   </si>
@@ -58,91 +58,139 @@
     <t>CDNT</t>
   </si>
   <si>
-    <t>DTVC</t>
-  </si>
-  <si>
-    <t>Delito vs TPúb</t>
-  </si>
-  <si>
-    <t>2020-01-12</t>
-  </si>
-  <si>
-    <t>Partido microteléfono de una EP. Calle 6ta, Doble Vía. Comercial Vigía Sur de Santa Clara</t>
-  </si>
-  <si>
-    <t>Santa Clara</t>
-  </si>
-  <si>
-    <t/>
+    <t>DTHO</t>
+  </si>
+  <si>
+    <t>Delito vs PExt</t>
+  </si>
+  <si>
+    <t>2020-03-11</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte de FON aérea. Localidad Arroyo seco</t>
+  </si>
+  <si>
+    <t>Mayarí</t>
+  </si>
+  <si>
+    <t>Fibra óptica-1</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>DTVC-01-20-0004</t>
-  </si>
-  <si>
-    <t>2020-05-02</t>
-  </si>
-  <si>
-    <t>Sustracción de microteléfono a una EP. Carretera a Sagua km 10</t>
-  </si>
-  <si>
-    <t>DTVC-05-20-0069</t>
-  </si>
-  <si>
-    <t>2020-05-12</t>
-  </si>
-  <si>
-    <t>Sustraido microteléfono de una EP. Calle Juan Bruno Zayas, entre Feria y Dámaso Rodriguez. Portal de la Bodega Potrero Grande</t>
-  </si>
-  <si>
-    <t>Manicaragua</t>
-  </si>
-  <si>
-    <t>DTVC-05-20-0076</t>
-  </si>
-  <si>
-    <t>2020-08-04</t>
-  </si>
-  <si>
-    <t>Desprendido el microteléfono de una EP. Consejo Popular  Quintín Bandera</t>
-  </si>
-  <si>
-    <t>Corralillo</t>
-  </si>
-  <si>
-    <t>DTVC-08-20-0147</t>
-  </si>
-  <si>
-    <t>2020-08-05</t>
-  </si>
-  <si>
-    <t>Fracturado el microteléfono de una EP. Calle J. Paneca No . 33 e/t Martí y Camilo</t>
-  </si>
-  <si>
-    <t>Camajuaní</t>
-  </si>
-  <si>
-    <t>DTVC-08-20-0150</t>
-  </si>
-  <si>
-    <t>2020-08-08</t>
-  </si>
-  <si>
-    <t>Sustraccióm de la antena exterior a una EP(GSM). Consejo Popular La Yaya</t>
-  </si>
-  <si>
-    <t>DTVC-08-20-0152</t>
-  </si>
-  <si>
-    <t>2020-09-09</t>
-  </si>
-  <si>
-    <t>Vandalizada una EP. Portal de correo de Sierra Morena</t>
-  </si>
-  <si>
-    <t>DTVC-09-20-0184</t>
+    <t>DTHO-03-20-0032</t>
+  </si>
+  <si>
+    <t>2020-05-13</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por corte y sustracción de bajante telefónico. Calle Nicio García, No. 230,  entre 19 y 25</t>
+  </si>
+  <si>
+    <t>Holguín</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-20</t>
+  </si>
+  <si>
+    <t>DTHO-05-20-0046</t>
+  </si>
+  <si>
+    <t>2020-06-20</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por corte intensional de FO. Carretera vía San Andrés.Entrada a Purnio</t>
+  </si>
+  <si>
+    <t>DTHO-06-20-0059</t>
+  </si>
+  <si>
+    <t>2020-07-10</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por corte y sustracción de bajante telefónico. Calle 26 de Julio,  No. 143</t>
+  </si>
+  <si>
+    <t>Calixto García</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-48</t>
+  </si>
+  <si>
+    <t>DTHO-07-20-0063</t>
+  </si>
+  <si>
+    <t>2020-07-14</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por corte y sustracción de bajante telefónico. Calle 13 de Marzo</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-200</t>
+  </si>
+  <si>
+    <t>DTHO-07-20-0065</t>
+  </si>
+  <si>
+    <t>2020-07-26</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por Gabinete Distribución vandalizado. Carretera a San Germán. Rpto. 26 de Julio</t>
+  </si>
+  <si>
+    <t>Gabinetes-1</t>
+  </si>
+  <si>
+    <t>DTHO-07-20-0068</t>
+  </si>
+  <si>
+    <t>2020-08-28</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por sustracción de cable de 400 pares. Carretera central Vía Las Tunas. Entre 36 y 38</t>
+  </si>
+  <si>
+    <t>Cable telefónico-60</t>
+  </si>
+  <si>
+    <t>DTHO-08-20-0084</t>
+  </si>
+  <si>
+    <t>2020-09-03</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Localidad de San Germán. La Loma</t>
+  </si>
+  <si>
+    <t>Urbano Noris</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-410</t>
+  </si>
+  <si>
+    <t>DTHO-09-20-0086</t>
+  </si>
+  <si>
+    <t>2020-11-12</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Vía las Tunas</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-50</t>
+  </si>
+  <si>
+    <t>DTHO-11-20-0114</t>
+  </si>
+  <si>
+    <t>2020-11-24</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Carretera Central . Rpto. Oscar Lucero</t>
+  </si>
+  <si>
+    <t>DTHO-11-20-0116</t>
   </si>
 </sst>
 </file>
@@ -633,7 +681,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <sheetPr/>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -711,13 +759,13 @@
         <v>18</v>
       </c>
       <c r="F2" s="3">
-        <v>46.42</v>
+        <v>0</v>
       </c>
       <c r="G2" s="3">
-        <v>66.28</v>
+        <v>0</v>
       </c>
       <c r="H2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>19</v>
@@ -750,19 +798,19 @@
         <v>23</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F3" s="6">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="G3" s="6">
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="H3" s="6">
         <v>1</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
@@ -775,7 +823,7 @@
         <v>20</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -786,22 +834,22 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F4" s="6">
-        <v>43.11</v>
+        <v>78.9</v>
       </c>
       <c r="G4" s="6">
-        <v>0</v>
+        <v>158.6</v>
       </c>
       <c r="H4" s="6">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>19</v>
@@ -817,7 +865,7 @@
         <v>20</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
@@ -828,13 +876,13 @@
         <v>15</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" s="6">
         <v>0</v>
@@ -846,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
@@ -859,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -870,25 +918,25 @@
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F6" s="6">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="G6" s="6">
-        <v>0</v>
+        <v>257.6</v>
       </c>
       <c r="H6" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6" t="s">
@@ -901,7 +949,7 @@
         <v>20</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7">
@@ -912,13 +960,13 @@
         <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F7" s="6">
         <v>0</v>
@@ -927,10 +975,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="6">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6" t="s">
@@ -943,49 +991,175 @@
         <v>20</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="C8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="6">
         <v>0</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="6">
+        <v>394.23</v>
+      </c>
+      <c r="H8" s="6">
+        <v>146</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="6">
         <v>0</v>
       </c>
-      <c r="H8" s="9">
+      <c r="G9" s="6">
+        <v>6.52</v>
+      </c>
+      <c r="H9" s="6">
+        <v>2</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="6">
+        <v>25</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
         <v>1</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>42</v>
+      <c r="I10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="9">
+        <v>25</v>
+      </c>
+      <c r="G11" s="9">
+        <v>82.9</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
annadido sistema identificativo con subida de imagenes
</commit_message>
<xml_diff>
--- a/src/informesGenerados/HechosParaUnidadOrganizativa.xlsx
+++ b/src/informesGenerados/HechosParaUnidadOrganizativa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>UOrg</t>
   </si>
@@ -58,91 +58,139 @@
     <t>CDNT</t>
   </si>
   <si>
-    <t>DTVC</t>
-  </si>
-  <si>
-    <t>Delito vs TPúb</t>
-  </si>
-  <si>
-    <t>2020-01-12</t>
-  </si>
-  <si>
-    <t>Partido microteléfono de una EP. Calle 6ta, Doble Vía. Comercial Vigía Sur de Santa Clara</t>
-  </si>
-  <si>
-    <t>Santa Clara</t>
-  </si>
-  <si>
-    <t/>
+    <t>DTHO</t>
+  </si>
+  <si>
+    <t>Delito vs PExt</t>
+  </si>
+  <si>
+    <t>2020-03-11</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte de FON aérea. Localidad Arroyo seco</t>
+  </si>
+  <si>
+    <t>Mayarí</t>
+  </si>
+  <si>
+    <t>Fibra óptica-1</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>DTVC-01-20-0004</t>
-  </si>
-  <si>
-    <t>2020-05-02</t>
-  </si>
-  <si>
-    <t>Sustracción de microteléfono a una EP. Carretera a Sagua km 10</t>
-  </si>
-  <si>
-    <t>DTVC-05-20-0069</t>
-  </si>
-  <si>
-    <t>2020-05-12</t>
-  </si>
-  <si>
-    <t>Sustraido microteléfono de una EP. Calle Juan Bruno Zayas, entre Feria y Dámaso Rodriguez. Portal de la Bodega Potrero Grande</t>
-  </si>
-  <si>
-    <t>Manicaragua</t>
-  </si>
-  <si>
-    <t>DTVC-05-20-0076</t>
-  </si>
-  <si>
-    <t>2020-08-04</t>
-  </si>
-  <si>
-    <t>Desprendido el microteléfono de una EP. Consejo Popular  Quintín Bandera</t>
-  </si>
-  <si>
-    <t>Corralillo</t>
-  </si>
-  <si>
-    <t>DTVC-08-20-0147</t>
-  </si>
-  <si>
-    <t>2020-08-05</t>
-  </si>
-  <si>
-    <t>Fracturado el microteléfono de una EP. Calle J. Paneca No . 33 e/t Martí y Camilo</t>
-  </si>
-  <si>
-    <t>Camajuaní</t>
-  </si>
-  <si>
-    <t>DTVC-08-20-0150</t>
-  </si>
-  <si>
-    <t>2020-08-08</t>
-  </si>
-  <si>
-    <t>Sustraccióm de la antena exterior a una EP(GSM). Consejo Popular La Yaya</t>
-  </si>
-  <si>
-    <t>DTVC-08-20-0152</t>
-  </si>
-  <si>
-    <t>2020-09-09</t>
-  </si>
-  <si>
-    <t>Vandalizada una EP. Portal de correo de Sierra Morena</t>
-  </si>
-  <si>
-    <t>DTVC-09-20-0184</t>
+    <t>DTHO-03-20-0032</t>
+  </si>
+  <si>
+    <t>2020-05-13</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por corte y sustracción de bajante telefónico. Calle Nicio García, No. 230,  entre 19 y 25</t>
+  </si>
+  <si>
+    <t>Holguín</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-20</t>
+  </si>
+  <si>
+    <t>DTHO-05-20-0046</t>
+  </si>
+  <si>
+    <t>2020-06-20</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por corte intensional de FO. Carretera vía San Andrés.Entrada a Purnio</t>
+  </si>
+  <si>
+    <t>DTHO-06-20-0059</t>
+  </si>
+  <si>
+    <t>2020-07-10</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por corte y sustracción de bajante telefónico. Calle 26 de Julio,  No. 143</t>
+  </si>
+  <si>
+    <t>Calixto García</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-48</t>
+  </si>
+  <si>
+    <t>DTHO-07-20-0063</t>
+  </si>
+  <si>
+    <t>2020-07-14</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por corte y sustracción de bajante telefónico. Calle 13 de Marzo</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-200</t>
+  </si>
+  <si>
+    <t>DTHO-07-20-0065</t>
+  </si>
+  <si>
+    <t>2020-07-26</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior, por Gabinete Distribución vandalizado. Carretera a San Germán. Rpto. 26 de Julio</t>
+  </si>
+  <si>
+    <t>Gabinetes-1</t>
+  </si>
+  <si>
+    <t>DTHO-07-20-0068</t>
+  </si>
+  <si>
+    <t>2020-08-28</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por sustracción de cable de 400 pares. Carretera central Vía Las Tunas. Entre 36 y 38</t>
+  </si>
+  <si>
+    <t>Cable telefónico-60</t>
+  </si>
+  <si>
+    <t>DTHO-08-20-0084</t>
+  </si>
+  <si>
+    <t>2020-09-03</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Localidad de San Germán. La Loma</t>
+  </si>
+  <si>
+    <t>Urbano Noris</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-410</t>
+  </si>
+  <si>
+    <t>DTHO-09-20-0086</t>
+  </si>
+  <si>
+    <t>2020-11-12</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Vía las Tunas</t>
+  </si>
+  <si>
+    <t>Bajante telefónico-50</t>
+  </si>
+  <si>
+    <t>DTHO-11-20-0114</t>
+  </si>
+  <si>
+    <t>2020-11-24</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Carretera Central . Rpto. Oscar Lucero</t>
+  </si>
+  <si>
+    <t>DTHO-11-20-0116</t>
   </si>
 </sst>
 </file>
@@ -633,7 +681,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <sheetPr/>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -711,13 +759,13 @@
         <v>18</v>
       </c>
       <c r="F2" s="3">
-        <v>46.42</v>
+        <v>0</v>
       </c>
       <c r="G2" s="3">
-        <v>66.28</v>
+        <v>0</v>
       </c>
       <c r="H2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>19</v>
@@ -750,19 +798,19 @@
         <v>23</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F3" s="6">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="G3" s="6">
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="H3" s="6">
         <v>1</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
@@ -775,7 +823,7 @@
         <v>20</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -786,22 +834,22 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F4" s="6">
-        <v>43.11</v>
+        <v>78.9</v>
       </c>
       <c r="G4" s="6">
-        <v>0</v>
+        <v>158.6</v>
       </c>
       <c r="H4" s="6">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>19</v>
@@ -817,7 +865,7 @@
         <v>20</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
@@ -828,13 +876,13 @@
         <v>15</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" s="6">
         <v>0</v>
@@ -846,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
@@ -859,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -870,25 +918,25 @@
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F6" s="6">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="G6" s="6">
-        <v>0</v>
+        <v>257.6</v>
       </c>
       <c r="H6" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6" t="s">
@@ -901,7 +949,7 @@
         <v>20</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7">
@@ -912,13 +960,13 @@
         <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F7" s="6">
         <v>0</v>
@@ -927,10 +975,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="6">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6" t="s">
@@ -943,49 +991,175 @@
         <v>20</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="C8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="6">
         <v>0</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="6">
+        <v>394.23</v>
+      </c>
+      <c r="H8" s="6">
+        <v>146</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="6">
         <v>0</v>
       </c>
-      <c r="H8" s="9">
+      <c r="G9" s="6">
+        <v>6.52</v>
+      </c>
+      <c r="H9" s="6">
+        <v>2</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="6">
+        <v>25</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
         <v>1</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>42</v>
+      <c r="I10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="9">
+        <v>25</v>
+      </c>
+      <c r="G11" s="9">
+        <v>82.9</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>